<commit_message>
update sensitivity results final 0606
</commit_message>
<xml_diff>
--- a/Plotting/Latex/filtered_data_sensitivity.xlsx
+++ b/Plotting/Latex/filtered_data_sensitivity.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,46 +707,36 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Conventional cracker existing</t>
+          <t>Conventional cracker with \acs{CC}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>t naphtha/h</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
+          <t>\% captured</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -758,8 +748,10 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M6" t="n">
-        <v>0</v>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -771,8 +763,10 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P6" t="n">
-        <v>0</v>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -791,7 +785,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Electric cracker</t>
+          <t>Conventional cracker existing</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -799,50 +793,74 @@
           <t>t naphtha/h</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0</v>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -851,36 +869,46 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Conventional reformer</t>
+          <t>Conventional cracker existing with \acs{CC}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MW gas</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>895</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>708</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>\% captured</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -892,10 +920,8 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="M8" t="n">
+        <v>0</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -907,10 +933,8 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="P8" t="n">
+        <v>0</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -929,82 +953,58 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Conventional reformer existing</t>
+          <t>Electric cracker</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MW gas</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>t naphtha/h</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Electric reformer</t>
+          <t>Conventional reformer</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1022,49 +1022,67 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>760</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>896</v>
       </c>
       <c r="F10" t="n">
-        <v>745</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>691</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>895</v>
       </c>
       <c r="I10" t="n">
-        <v>733</v>
-      </c>
-      <c r="J10" t="n">
-        <v>744</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>746</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>739</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -1073,76 +1091,76 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Electric reformer existing</t>
+          <t>Conventional reformer with \acs{CC}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MW gas</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>\% captured</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>81</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>77</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K11" t="n">
-        <v>744</v>
-      </c>
-      <c r="L11" t="n">
-        <v>744</v>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="N11" t="n">
-        <v>746</v>
-      </c>
-      <c r="O11" t="n">
-        <v>746</v>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q11" t="n">
-        <v>739</v>
-      </c>
-      <c r="R11" t="n">
-        <v>739</v>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1151,58 +1169,82 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>\acs{AEC}</t>
+          <t>Conventional reformer existing</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MW electric</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>238</v>
-      </c>
-      <c r="H12" t="n">
-        <v>460</v>
-      </c>
-      <c r="I12" t="n">
-        <v>190</v>
+          <t>MW gas</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="n">
-        <v>11</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="M12" t="n">
-        <v>140</v>
-      </c>
-      <c r="N12" t="n">
-        <v>127</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P12" t="n">
-        <v>192</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>75</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -1211,12 +1253,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>\acs{AEC} existing</t>
+          <t>Conventional reformer existing with \acs{CC}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MW electric</t>
+          <t>\% captured</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1249,40 +1291,44 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J13" t="n">
+        <v>0</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="L13" t="n">
-        <v>11</v>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N13" t="n">
-        <v>140</v>
-      </c>
-      <c r="O13" t="n">
-        <v>267</v>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q13" t="n">
-        <v>192</v>
-      </c>
-      <c r="R13" t="n">
-        <v>268</v>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1291,34 +1337,34 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>\acs{HB} process</t>
+          <t>Electric reformer</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MW hydrogen</t>
+          <t>MW gas</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>828</v>
+        <v>760</v>
       </c>
       <c r="E14" t="n">
-        <v>805</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>803</v>
+        <v>745</v>
       </c>
       <c r="G14" t="n">
-        <v>841</v>
+        <v>758</v>
       </c>
       <c r="H14" t="n">
-        <v>830</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>803</v>
+        <v>731</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1327,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1336,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>739</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
@@ -1351,12 +1397,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>\acs{HB} process existing</t>
+          <t>Electric reformer existing</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MW hydrogen</t>
+          <t>MW gas</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1389,32 +1435,38 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J15" t="n">
-        <v>813</v>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="K15" t="n">
-        <v>813</v>
+        <v>744</v>
       </c>
       <c r="L15" t="n">
-        <v>813</v>
-      </c>
-      <c r="M15" t="n">
-        <v>813</v>
+        <v>744</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="N15" t="n">
-        <v>813</v>
+        <v>744</v>
       </c>
       <c r="O15" t="n">
-        <v>813</v>
-      </c>
-      <c r="P15" t="n">
-        <v>813</v>
+        <v>744</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q15" t="n">
-        <v>813</v>
+        <v>739</v>
       </c>
       <c r="R15" t="n">
-        <v>813</v>
+        <v>739</v>
       </c>
     </row>
     <row r="16">
@@ -1423,12 +1475,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Methanol synthesis from syngas</t>
+          <t>\acs{AEC}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>t syngas/h</t>
+          <t>MW electric</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1441,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1456,22 +1508,22 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
@@ -1483,12 +1535,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Direct methanol synthesis from \ce{CO2}</t>
+          <t>\acs{AEC} existing</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>t \ce{CO2}/h</t>
+          <t>MW electric</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1496,44 +1548,58 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1541,10 +1607,10 @@
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18">
@@ -1553,34 +1619,34 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>\acs{MTO}</t>
+          <t>\acs{HB} process</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>t methanol/h</t>
+          <t>MW hydrogen</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>253</v>
+        <v>827</v>
       </c>
       <c r="E18" t="n">
-        <v>36</v>
+        <v>806</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="G18" t="n">
-        <v>496</v>
+        <v>827</v>
       </c>
       <c r="H18" t="n">
-        <v>484</v>
+        <v>805</v>
       </c>
       <c r="I18" t="n">
-        <v>377</v>
+        <v>803</v>
       </c>
       <c r="J18" t="n">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1589,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -1598,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
@@ -1613,12 +1679,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>\acs{MTO} existing</t>
+          <t>\acs{HB} process existing</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>t methanol/h</t>
+          <t>MW hydrogen</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1651,38 +1717,32 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="J19" t="n">
+        <v>813</v>
       </c>
       <c r="K19" t="n">
-        <v>253</v>
+        <v>813</v>
       </c>
       <c r="L19" t="n">
-        <v>253</v>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>813</v>
+      </c>
+      <c r="M19" t="n">
+        <v>813</v>
       </c>
       <c r="N19" t="n">
-        <v>496</v>
+        <v>813</v>
       </c>
       <c r="O19" t="n">
-        <v>496</v>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>813</v>
+      </c>
+      <c r="P19" t="n">
+        <v>813</v>
       </c>
       <c r="Q19" t="n">
-        <v>496</v>
+        <v>813</v>
       </c>
       <c r="R19" t="n">
-        <v>496</v>
+        <v>813</v>
       </c>
     </row>
     <row r="20">
@@ -1691,12 +1751,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>\acs{EDH}</t>
+          <t>Methanol synthesis from syngas</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>t ethanol/h</t>
+          <t>t syngas/h</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1751,25 +1811,29 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>\acs{PDH}</t>
+          <t>Direct methanol synthesis from \ce{CO2}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>t propane/h</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>157</v>
+          <t>t \ce{CO2}/h</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E21" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>139</v>
-      </c>
-      <c r="G21" t="n">
-        <v>64</v>
+        <v>0</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1777,8 +1841,10 @@
       <c r="I21" t="n">
         <v>0</v>
       </c>
-      <c r="J21" t="n">
-        <v>157</v>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -1786,8 +1852,10 @@
       <c r="L21" t="n">
         <v>0</v>
       </c>
-      <c r="M21" t="n">
-        <v>64</v>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="N21" t="n">
         <v>0</v>
@@ -1795,8 +1863,10 @@
       <c r="O21" t="n">
         <v>0</v>
       </c>
-      <c r="P21" t="n">
-        <v>64</v>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
@@ -1811,76 +1881,58 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>\acs{PDH} existing</t>
+          <t>\acs{MTO}</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>t propane/h</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>t methanol/h</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>253</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>253</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>253</v>
       </c>
       <c r="K22" t="n">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="L22" t="n">
-        <v>157</v>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>253</v>
       </c>
       <c r="N22" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>64</v>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>496</v>
       </c>
       <c r="Q22" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1889,58 +1941,76 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>\acs{MPW}-to-methanol</t>
+          <t>\acs{MTO} existing</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>t MPW/h</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>172</v>
-      </c>
-      <c r="E23" t="n">
-        <v>25</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>338</v>
-      </c>
-      <c r="H23" t="n">
-        <v>329</v>
-      </c>
-      <c r="I23" t="n">
-        <v>256</v>
-      </c>
-      <c r="J23" t="n">
-        <v>172</v>
+          <t>t methanol/h</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
-        <v>338</v>
+        <v>280</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>338</v>
+        <v>253</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>496</v>
       </c>
     </row>
     <row r="24">
@@ -1949,76 +2019,58 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>\acs{MPW}-to-methanol existing</t>
+          <t>\acs{EDH}</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>t MPW/h</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>t ethanol/h</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>172</v>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>338</v>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2027,68 +2079,58 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>\ce{CO2} electrolysis</t>
+          <t>\acs{PDH}</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>t \ce{CO2}/h</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>t propane/h</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>157</v>
       </c>
       <c r="E25" t="n">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="F25" t="n">
-        <v>162</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>139</v>
+      </c>
+      <c r="G25" t="n">
+        <v>157</v>
       </c>
       <c r="H25" t="n">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="I25" t="n">
-        <v>156</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>157</v>
+      </c>
+      <c r="J25" t="n">
+        <v>157</v>
       </c>
       <c r="K25" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>60</v>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>157</v>
       </c>
       <c r="N25" t="n">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>39</v>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>64</v>
       </c>
       <c r="Q25" t="n">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="R25" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2097,12 +2139,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>\ce{CO2} electrolysis existing</t>
+          <t>\acs{PDH} existing</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>t \ce{CO2}/h</t>
+          <t>t propane/h</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2140,39 +2182,33 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K26" t="n">
+        <v>157</v>
       </c>
       <c r="L26" t="n">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="N26" t="n">
+        <v>157</v>
       </c>
       <c r="O26" t="n">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="Q26" t="n">
+        <v>64</v>
       </c>
       <c r="R26" t="n">
-        <v>111</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
@@ -2181,43 +2217,43 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>\acs{ASU}</t>
+          <t>\acs{MPW}-to-methanol</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MW electricity</t>
+          <t>t MPW/h</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>29</v>
+        <v>172</v>
       </c>
       <c r="H27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
@@ -2226,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>28</v>
+        <v>338</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
@@ -2241,76 +2277,58 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>\acs{ASU} existing</t>
+          <t>\acs{MPW}-to-methanol with \acs{CC}</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MW electricity</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>\% captured</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="L28" t="n">
-        <v>28</v>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
       </c>
       <c r="N28" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>28</v>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>3</v>
       </c>
       <c r="Q28" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="R28" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2319,58 +2337,76 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Gas-fired boiler</t>
+          <t>\acs{MPW}-to-methanol existing</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MW gas</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>375</v>
-      </c>
-      <c r="E29" t="n">
-        <v>401</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>128</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" t="n">
-        <v>367</v>
+          <t>t MPW/h</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" t="n">
-        <v>123</v>
+        <v>190</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>122</v>
+        <v>172</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30">
@@ -2379,12 +2415,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Gas-fired boiler existing</t>
+          <t>\acs{MPW}-to-methanol existing with \acs{CC}</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MW gas</t>
+          <t>\% captured</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2423,10 +2459,10 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>367</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>367</v>
+        <v>0</v>
       </c>
       <c r="M30" t="inlineStr">
         <is>
@@ -2434,10 +2470,10 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -2445,10 +2481,10 @@
         </is>
       </c>
       <c r="Q30" t="n">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="R30" t="n">
-        <v>122</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31">
@@ -2457,58 +2493,68 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Electric boiler</t>
+          <t>\ce{CO2} electrolysis</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MW electricity</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>294</v>
+          <t>t \ce{CO2}/h</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E31" t="n">
-        <v>432</v>
+        <v>146</v>
       </c>
       <c r="F31" t="n">
-        <v>252</v>
-      </c>
-      <c r="G31" t="n">
-        <v>67</v>
+        <v>162</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="H31" t="n">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I31" t="n">
-        <v>123</v>
-      </c>
-      <c r="J31" t="n">
-        <v>293</v>
+        <v>138</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="K31" t="n">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>64</v>
+        <v>32</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="O31" t="n">
-        <v>52</v>
-      </c>
-      <c r="P31" t="n">
-        <v>97</v>
+        <v>38</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="R31" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
@@ -2517,12 +2563,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Electric boiler existing</t>
+          <t>\ce{CO2} electrolysis existing</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MW electricity</t>
+          <t>t \ce{CO2}/h</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2560,33 +2606,39 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K32" t="n">
-        <v>293</v>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="L32" t="n">
-        <v>383</v>
+        <v>129</v>
       </c>
       <c r="M32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="N32" t="n">
-        <v>64</v>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O32" t="n">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q32" t="n">
-        <v>97</v>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="R32" t="n">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
@@ -2595,55 +2647,55 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Ammonia tank</t>
+          <t>\acs{ASU}</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>tonne</t>
+          <t>MW electricity</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4817</v>
+        <v>28</v>
       </c>
       <c r="E33" t="n">
-        <v>1182</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="G33" t="n">
-        <v>7343</v>
+        <v>28</v>
       </c>
       <c r="H33" t="n">
-        <v>5487</v>
+        <v>4</v>
       </c>
       <c r="I33" t="n">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="J33" t="n">
-        <v>2915</v>
+        <v>28</v>
       </c>
       <c r="K33" t="n">
-        <v>6201</v>
+        <v>0</v>
       </c>
       <c r="L33" t="n">
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>5178</v>
+        <v>28</v>
       </c>
       <c r="N33" t="n">
-        <v>3938</v>
+        <v>0</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>4513</v>
+        <v>28</v>
       </c>
       <c r="Q33" t="n">
-        <v>4602</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
         <v>0</v>
@@ -2655,12 +2707,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ammonia tank existing</t>
+          <t>\acs{ASU} existing</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>tonne</t>
+          <t>MW electricity</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2699,10 +2751,10 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>2915</v>
+        <v>28</v>
       </c>
       <c r="L34" t="n">
-        <v>9116</v>
+        <v>28</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
@@ -2710,10 +2762,10 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>5178</v>
+        <v>28</v>
       </c>
       <c r="O34" t="n">
-        <v>9116</v>
+        <v>28</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -2721,10 +2773,10 @@
         </is>
       </c>
       <c r="Q34" t="n">
-        <v>4513</v>
+        <v>28</v>
       </c>
       <c r="R34" t="n">
-        <v>9116</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35">
@@ -2733,55 +2785,55 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Li-ion battery</t>
+          <t>Gas-fired boiler</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>MW gas</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1222</v>
+        <v>368</v>
       </c>
       <c r="E35" t="n">
-        <v>4508</v>
+        <v>401</v>
       </c>
       <c r="F35" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>1217</v>
+        <v>368</v>
       </c>
       <c r="H35" t="n">
-        <v>5736</v>
+        <v>401</v>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>1520</v>
+        <v>355</v>
       </c>
       <c r="K35" t="n">
-        <v>6414</v>
+        <v>11</v>
       </c>
       <c r="L35" t="n">
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>1643</v>
+        <v>367</v>
       </c>
       <c r="N35" t="n">
-        <v>6414</v>
+        <v>0</v>
       </c>
       <c r="O35" t="n">
         <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>1639</v>
+        <v>122</v>
       </c>
       <c r="Q35" t="n">
-        <v>6414</v>
+        <v>0</v>
       </c>
       <c r="R35" t="n">
         <v>0</v>
@@ -2793,12 +2845,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Li-ion battery existing</t>
+          <t>Gas-fired boiler existing</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>MW gas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2837,10 +2889,10 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>1520</v>
+        <v>355</v>
       </c>
       <c r="L36" t="n">
-        <v>7934</v>
+        <v>367</v>
       </c>
       <c r="M36" t="inlineStr">
         <is>
@@ -2848,10 +2900,10 @@
         </is>
       </c>
       <c r="N36" t="n">
-        <v>1643</v>
+        <v>367</v>
       </c>
       <c r="O36" t="n">
-        <v>8057</v>
+        <v>367</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -2859,10 +2911,10 @@
         </is>
       </c>
       <c r="Q36" t="n">
-        <v>1639</v>
+        <v>122</v>
       </c>
       <c r="R36" t="n">
-        <v>8053</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37">
@@ -2871,58 +2923,58 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>\ce{CO2} buffer storage</t>
+          <t>Electric boiler</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>tonne</t>
+          <t>MW electricity</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>190</v>
+        <v>293</v>
       </c>
       <c r="E37" t="n">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="F37" t="n">
-        <v>1008</v>
+        <v>251</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>291</v>
       </c>
       <c r="H37" t="n">
-        <v>6321</v>
+        <v>246</v>
       </c>
       <c r="I37" t="n">
-        <v>46</v>
+        <v>294</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>293</v>
       </c>
       <c r="K37" t="n">
-        <v>4478</v>
+        <v>0</v>
       </c>
       <c r="L37" t="n">
         <v>0</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>293</v>
       </c>
       <c r="N37" t="n">
-        <v>9867</v>
+        <v>0</v>
       </c>
       <c r="O37" t="n">
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>2135</v>
+        <v>97</v>
       </c>
       <c r="Q37" t="n">
-        <v>7669</v>
+        <v>0</v>
       </c>
       <c r="R37" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38">
@@ -2931,12 +2983,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>\ce{CO2} buffer storage existing</t>
+          <t>Electric boiler existing</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>tonne</t>
+          <t>MW electricity</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2974,26 +3026,22 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K38" t="n">
+        <v>293</v>
       </c>
       <c r="L38" t="n">
-        <v>4478</v>
+        <v>293</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="N38" t="n">
+        <v>293</v>
       </c>
       <c r="O38" t="n">
-        <v>9867</v>
+        <v>293</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
@@ -3001,10 +3049,10 @@
         </is>
       </c>
       <c r="Q38" t="n">
-        <v>2135</v>
+        <v>97</v>
       </c>
       <c r="R38" t="n">
-        <v>9805</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39">
@@ -3013,55 +3061,55 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Hydrogen tank</t>
+          <t>Ammonia tank</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>tonne</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>443</v>
+        <v>4686</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1661</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>128</v>
+        <v>4737</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>3358</v>
       </c>
       <c r="K39" t="n">
-        <v>757</v>
+        <v>5389</v>
       </c>
       <c r="L39" t="n">
         <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>155</v>
+        <v>3656</v>
       </c>
       <c r="N39" t="n">
-        <v>8463</v>
+        <v>5433</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
       </c>
       <c r="P39" t="n">
-        <v>270</v>
+        <v>4513</v>
       </c>
       <c r="Q39" t="n">
-        <v>8471</v>
+        <v>4602</v>
       </c>
       <c r="R39" t="n">
         <v>0</v>
@@ -3073,12 +3121,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Hydrogen tank existing</t>
+          <t>Ammonia tank existing</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MWh</t>
+          <t>tonne</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3116,13 +3164,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K40" t="n">
+        <v>3358</v>
       </c>
       <c r="L40" t="n">
-        <v>757</v>
+        <v>8747</v>
       </c>
       <c r="M40" t="inlineStr">
         <is>
@@ -3130,10 +3176,10 @@
         </is>
       </c>
       <c r="N40" t="n">
-        <v>155</v>
+        <v>3656</v>
       </c>
       <c r="O40" t="n">
-        <v>8618</v>
+        <v>9089</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
@@ -3141,10 +3187,10 @@
         </is>
       </c>
       <c r="Q40" t="n">
-        <v>270</v>
+        <v>4513</v>
       </c>
       <c r="R40" t="n">
-        <v>8741</v>
+        <v>9116</v>
       </c>
     </row>
     <row r="41">
@@ -3153,55 +3199,55 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ethylene tank</t>
+          <t>Li-ion battery</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>tonne</t>
+          <t>MWh</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1240</v>
       </c>
       <c r="E41" t="n">
-        <v>499</v>
+        <v>4957</v>
       </c>
       <c r="F41" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>1240</v>
       </c>
       <c r="H41" t="n">
-        <v>5348</v>
+        <v>5423</v>
       </c>
       <c r="I41" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>1470</v>
       </c>
       <c r="K41" t="n">
-        <v>6647</v>
+        <v>6414</v>
       </c>
       <c r="L41" t="n">
         <v>0</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>1432</v>
       </c>
       <c r="N41" t="n">
-        <v>499</v>
+        <v>6414</v>
       </c>
       <c r="O41" t="n">
         <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
+        <v>1639</v>
       </c>
       <c r="Q41" t="n">
-        <v>5336</v>
+        <v>6414</v>
       </c>
       <c r="R41" t="n">
         <v>0</v>
@@ -3213,12 +3259,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ethylene tank existing</t>
+          <t>Li-ion battery existing</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>tonne</t>
+          <t>MWh</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3256,13 +3302,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="K42" t="n">
+        <v>1470</v>
       </c>
       <c r="L42" t="n">
-        <v>6647</v>
+        <v>7884</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -3270,23 +3314,21 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>1432</v>
       </c>
       <c r="O42" t="n">
-        <v>499</v>
+        <v>7846</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="Q42" t="n">
+        <v>1639</v>
       </c>
       <c r="R42" t="n">
-        <v>5336</v>
+        <v>8053</v>
       </c>
     </row>
     <row r="43">
@@ -3295,7 +3337,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Propylene tank</t>
+          <t>\ce{CO2} buffer storage</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3307,25 +3349,25 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>6961</v>
+        <v>1810</v>
       </c>
       <c r="F43" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>2212</v>
+        <v>1887</v>
       </c>
       <c r="I43" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>2633</v>
+        <v>1618</v>
       </c>
       <c r="L43" t="n">
         <v>0</v>
@@ -3334,16 +3376,16 @@
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>7561</v>
+        <v>117</v>
       </c>
       <c r="O43" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>2135</v>
       </c>
       <c r="Q43" t="n">
-        <v>498</v>
+        <v>7669</v>
       </c>
       <c r="R43" t="n">
         <v>0</v>
@@ -3355,79 +3397,509 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>\ce{CO2} buffer storage existing</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L44" t="n">
+        <v>1618</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O44" t="n">
+        <v>117</v>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q44" t="n">
+        <v>2135</v>
+      </c>
+      <c r="R44" t="n">
+        <v>9805</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Hydrogen tank</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>MWh</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>69</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>69</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>494</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>694</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>270</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>8471</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Hydrogen tank existing</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MWh</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L46" t="n">
+        <v>494</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O46" t="n">
+        <v>694</v>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q46" t="n">
+        <v>270</v>
+      </c>
+      <c r="R46" t="n">
+        <v>8741</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Ethylene tank</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>11418</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>7732</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>1133</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>477</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>5336</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Ethylene tank existing</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L48" t="n">
+        <v>1133</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O48" t="n">
+        <v>477</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R48" t="n">
+        <v>5336</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Propylene tank</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>tonne</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>500</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>984</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>6808</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>7147</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>498</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>Propylene tank existing</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>tonne</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L44" t="n">
-        <v>2633</v>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N44" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" t="n">
-        <v>7561</v>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R44" t="n">
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L50" t="n">
+        <v>6808</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O50" t="n">
+        <v>7147</v>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R50" t="n">
         <v>498</v>
       </c>
     </row>

</xml_diff>